<commit_message>
Updated various files in the project
</commit_message>
<xml_diff>
--- a/src/test/java/com/store/testdata/TestData.xlsx
+++ b/src/test/java/com/store/testdata/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOWMYA\Desktop\Selenium Training\EcommerceWebsite\src\test\java\com\store\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A518008-D5C7-4FAF-A593-E342C71992E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D12D834-8639-4043-8C6A-A469E032515D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -161,19 +161,19 @@
     <t>London</t>
   </si>
   <si>
-    <t>Warne</t>
-  </si>
-  <si>
-    <t>Rossy</t>
-  </si>
-  <si>
-    <t>8173678450</t>
-  </si>
-  <si>
-    <t>testaccount24@email.com</t>
-  </si>
-  <si>
-    <t>testaccount24</t>
+    <t>Marina</t>
+  </si>
+  <si>
+    <t>Avery</t>
+  </si>
+  <si>
+    <t>testaccount25@email.com</t>
+  </si>
+  <si>
+    <t>testaccount25</t>
+  </si>
+  <si>
+    <t>8173678441</t>
   </si>
 </sst>
 </file>
@@ -582,7 +582,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -640,10 +640,10 @@
         <v>45</v>
       </c>
       <c r="C2" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>48</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>22</v>
@@ -661,7 +661,7 @@
         <v>36</v>
       </c>
       <c r="J2" s="5" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>